<commit_message>
add stocks info and how to read from the config
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>炼化厂</t>
   </si>
@@ -55,22 +55,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>A</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qty</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>初始化数量（&lt;=10）</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -108,6 +92,130 @@
   </si>
   <si>
     <t>hello123456</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>仓库</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>原料库</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>聚氯乙烯</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>高苯聚氯乙烯</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成品库</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>塑料齿轮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>塑料连杆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>塑料外壳</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁质零件厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>热轧钢板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷轧钢板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁质齿轮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁质连杆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁质外壳</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝质零件厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>热轧铝板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷轧铝板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝质齿轮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝质连杆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝质外壳</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>品名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始库存基数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>停产上/下限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进货下限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生产/消耗速度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞机</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>汽车</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始库存上限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞机总装厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>汽车总装厂</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -467,7 +575,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -597,6 +705,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -726,7 +871,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -735,6 +880,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1085,24 +1263,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1115,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1132,18 +1310,18 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1318,47 +1496,970 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.25" customWidth="1"/>
+    <col min="7" max="8" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <f>D2*2</f>
+        <v>200</v>
+      </c>
+      <c r="G2" s="2">
+        <f>D2*2</f>
+        <v>200</v>
+      </c>
+      <c r="H2" s="2">
+        <f>G2*5</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2">
+        <v>50</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <f>D3*2</f>
+        <v>100</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="F3:H26" si="0">D3*2</f>
+        <v>100</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H36" si="1">G3*5</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E4" s="2">
+        <f>H4</f>
+        <v>20000</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E6" si="2">H5</f>
+        <v>10000</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2">
+        <v>500</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="2"/>
+        <v>5000</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <f>D7*2</f>
+        <v>20</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <f>D8*2</f>
+        <v>10</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E9" s="2">
+        <f>H9</f>
+        <v>20000</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" ref="E10:E11" si="3">H10</f>
+        <v>10000</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2">
+        <v>500</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="3"/>
+        <v>5000</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <f>D12*2</f>
+        <v>20</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <f>D13*2</f>
+        <v>10</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="5"/>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E14" s="2">
+        <f>H14</f>
+        <v>20000</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" ref="E15:E16" si="4">H15</f>
+        <v>10000</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="2">
+        <v>500</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2000</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <f>D17*2</f>
+        <v>4000</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" ref="F18:F25" si="5">D18*2</f>
+        <v>2000</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1200</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="5"/>
+        <v>2400</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="9">
+        <v>4000</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="5"/>
+        <v>8000</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="9">
+        <v>2000</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="5"/>
+        <v>4000</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="9">
+        <v>2000</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="5"/>
+        <v>4000</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="9">
+        <v>4000</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="5"/>
+        <v>8000</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="9">
+        <v>2400</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="5"/>
+        <v>4800</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" si="0"/>
+        <v>4800</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="9">
+        <v>3000</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="5"/>
+        <v>6000</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="13"/>
+      <c r="B26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="E26" s="9">
+        <f>H26</f>
+        <v>20</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="9">
+        <v>2500</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <f>D27*2</f>
+        <v>5000</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" ref="G27:H36" si="6">D27*2</f>
+        <v>5000</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1500</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" ref="F28:F35" si="7">D28*2</f>
+        <v>3000</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="6"/>
+        <v>3000</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1500</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="7"/>
+        <v>3000</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="6"/>
+        <v>3000</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="9">
+        <v>3000</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="7"/>
+        <v>6000</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="6"/>
+        <v>6000</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="9">
+        <v>4000</v>
+      </c>
+      <c r="E31" s="9">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="7"/>
+        <v>8000</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="6"/>
+        <v>8000</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="9">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="9">
+        <v>4000</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="7"/>
+        <v>8000</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="6"/>
+        <v>8000</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="9">
+        <v>3000</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="7"/>
+        <v>6000</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="6"/>
+        <v>6000</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="9">
+        <v>2500</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="7"/>
+        <v>5000</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="6"/>
+        <v>5000</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="13"/>
+      <c r="B36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="9">
+        <v>20</v>
+      </c>
+      <c r="E36" s="9">
+        <f>H36</f>
+        <v>200</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="9">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B27:B35"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
+  </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add init stocks by fname+wtype only
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -881,18 +881,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -913,6 +904,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1294,7 +1294,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1436,7 +1436,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -1450,7 +1450,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -1464,7 +1464,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -1498,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1526,27 +1526,27 @@
       <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="2">
@@ -1569,9 +1569,9 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="2">
@@ -1585,7 +1585,7 @@
         <v>100</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="F3:H26" si="0">D3*2</f>
+        <f t="shared" ref="G3:G26" si="0">D3*2</f>
         <v>100</v>
       </c>
       <c r="H3" s="2">
@@ -1594,11 +1594,11 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2">
@@ -1608,7 +1608,7 @@
         <f>H4</f>
         <v>20000</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G4" s="2">
@@ -1621,9 +1621,9 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="2">
@@ -1633,7 +1633,7 @@
         <f t="shared" ref="E5:E6" si="2">H5</f>
         <v>10000</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G5" s="2">
@@ -1646,9 +1646,9 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="2">
@@ -1658,7 +1658,7 @@
         <f t="shared" si="2"/>
         <v>5000</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G6" s="2">
@@ -1671,13 +1671,13 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="2">
@@ -1700,9 +1700,9 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="2">
@@ -1725,11 +1725,11 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="2">
@@ -1739,7 +1739,7 @@
         <f>H9</f>
         <v>20000</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G9" s="2">
@@ -1752,9 +1752,9 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="2">
@@ -1764,7 +1764,7 @@
         <f t="shared" ref="E10:E11" si="3">H10</f>
         <v>10000</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G10" s="2">
@@ -1777,9 +1777,9 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="2">
@@ -1789,7 +1789,7 @@
         <f t="shared" si="3"/>
         <v>5000</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="2">
@@ -1802,13 +1802,13 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="2">
@@ -1831,9 +1831,9 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="4" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2">
@@ -1856,11 +1856,11 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="5"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2">
@@ -1870,7 +1870,7 @@
         <f>H14</f>
         <v>20000</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G14" s="2">
@@ -1883,9 +1883,9 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2">
@@ -1895,7 +1895,7 @@
         <f t="shared" ref="E15:E16" si="4">H15</f>
         <v>10000</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G15" s="2">
@@ -1908,9 +1908,9 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2">
@@ -1920,7 +1920,7 @@
         <f t="shared" si="4"/>
         <v>5000</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G16" s="2">
@@ -1933,101 +1933,101 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="9">
-        <v>2000</v>
-      </c>
-      <c r="E17" s="9">
+      <c r="D17" s="6">
+        <v>3200</v>
+      </c>
+      <c r="E17" s="6">
         <v>0</v>
       </c>
       <c r="F17" s="2">
         <f>D17*2</f>
-        <v>4000</v>
-      </c>
-      <c r="G17" s="9">
+        <v>6400</v>
+      </c>
+      <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>6400</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="4" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="9">
-        <v>1000</v>
-      </c>
-      <c r="E18" s="9">
+      <c r="D18" s="6">
+        <v>1600</v>
+      </c>
+      <c r="E18" s="6">
         <v>0</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ref="F18:F25" si="5">D18*2</f>
-        <v>2000</v>
-      </c>
-      <c r="G18" s="9">
+        <v>3200</v>
+      </c>
+      <c r="G18" s="6">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>3200</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="9">
-        <v>1200</v>
-      </c>
-      <c r="E19" s="9">
+      <c r="D19" s="6">
+        <v>800</v>
+      </c>
+      <c r="E19" s="6">
         <v>0</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="5"/>
-        <v>2400</v>
-      </c>
-      <c r="G19" s="9">
+        <v>1600</v>
+      </c>
+      <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>2400</v>
+        <v>1600</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="1"/>
-        <v>12000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="4" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="6">
         <v>4000</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="6">
         <v>0</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="5"/>
         <v>8000</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="6">
         <f t="shared" si="0"/>
         <v>8000</v>
       </c>
@@ -2037,22 +2037,22 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="6">
         <v>2000</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="6">
         <v>0</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="5"/>
         <v>4000</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="6">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
@@ -2062,72 +2062,72 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="4" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="9">
-        <v>2000</v>
-      </c>
-      <c r="E22" s="9">
+      <c r="D22" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E22" s="6">
         <v>0</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="5"/>
-        <v>4000</v>
-      </c>
-      <c r="G22" s="9">
+        <v>2000</v>
+      </c>
+      <c r="G22" s="6">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="9">
-        <v>4000</v>
-      </c>
-      <c r="E23" s="9">
+      <c r="D23" s="6">
+        <v>4800</v>
+      </c>
+      <c r="E23" s="6">
         <v>0</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="5"/>
-        <v>8000</v>
-      </c>
-      <c r="G23" s="9">
+        <v>9600</v>
+      </c>
+      <c r="G23" s="6">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>9600</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="4" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="6">
         <v>2400</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="6">
         <v>0</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="5"/>
         <v>4800</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="6">
         <f t="shared" si="0"/>
         <v>4800</v>
       </c>
@@ -2137,49 +2137,49 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="9">
-        <v>3000</v>
-      </c>
-      <c r="E25" s="9">
+      <c r="D25" s="6">
+        <v>1200</v>
+      </c>
+      <c r="E25" s="6">
         <v>0</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="5"/>
-        <v>6000</v>
-      </c>
-      <c r="G25" s="9">
+        <v>2400</v>
+      </c>
+      <c r="G25" s="6">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>2400</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="13"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="6">
         <v>2</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="6">
         <f>H26</f>
         <v>20</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -2189,27 +2189,27 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="6">
         <v>2500</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="6">
         <v>0</v>
       </c>
       <c r="F27" s="2">
         <f>D27*2</f>
         <v>5000</v>
       </c>
-      <c r="G27" s="9">
-        <f t="shared" ref="G27:H36" si="6">D27*2</f>
+      <c r="G27" s="6">
+        <f t="shared" ref="G27:G36" si="6">D27*2</f>
         <v>5000</v>
       </c>
       <c r="H27" s="2">
@@ -2218,22 +2218,22 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="4" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="6">
         <v>1500</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="6">
         <v>0</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" ref="F28:F35" si="7">D28*2</f>
         <v>3000</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="6">
         <f t="shared" si="6"/>
         <v>3000</v>
       </c>
@@ -2243,22 +2243,22 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="4" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="6">
         <v>1500</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="6">
         <v>0</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="7"/>
         <v>3000</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="6">
         <f t="shared" si="6"/>
         <v>3000</v>
       </c>
@@ -2268,22 +2268,22 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="4" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="6">
         <v>3000</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="6">
         <v>0</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="7"/>
         <v>6000</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="6">
         <f t="shared" si="6"/>
         <v>6000</v>
       </c>
@@ -2293,22 +2293,22 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="4" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="6">
         <v>4000</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="6">
         <v>0</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="7"/>
         <v>8000</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="6">
         <f t="shared" si="6"/>
         <v>8000</v>
       </c>
@@ -2318,22 +2318,22 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="4" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="6">
         <v>1000</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="6">
         <v>0</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" si="7"/>
         <v>2000</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="6">
         <f t="shared" si="6"/>
         <v>2000</v>
       </c>
@@ -2343,22 +2343,22 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="4" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="6">
         <v>4000</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="6">
         <v>0</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" si="7"/>
         <v>8000</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="6">
         <f t="shared" si="6"/>
         <v>8000</v>
       </c>
@@ -2368,22 +2368,22 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="4" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="6">
         <v>3000</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="6">
         <v>0</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" si="7"/>
         <v>6000</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="6">
         <f t="shared" si="6"/>
         <v>6000</v>
       </c>
@@ -2393,22 +2393,22 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="4" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="6">
         <v>2500</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="6">
         <v>0</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="7"/>
         <v>5000</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="6">
         <f t="shared" si="6"/>
         <v>5000</v>
       </c>
@@ -2418,24 +2418,24 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="13"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="6">
         <v>20</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="6">
         <f>H36</f>
         <v>200</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="6">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
@@ -2446,6 +2446,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="A27:A36"/>
     <mergeCell ref="B27:B35"/>
     <mergeCell ref="A12:A16"/>
@@ -2453,12 +2459,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A17:A26"/>
     <mergeCell ref="B17:B25"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
connect real daily rate to log
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -963,14 +963,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -982,15 +979,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1619,10 +1619,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1648,8 +1648,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1673,8 +1673,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1700,8 +1700,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1725,8 +1725,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1750,10 +1750,10 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1779,8 +1779,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1804,8 +1804,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1831,8 +1831,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
@@ -1856,8 +1856,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
@@ -1881,10 +1881,10 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1910,8 +1910,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1935,8 +1935,8 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1962,8 +1962,8 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1987,8 +1987,8 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
@@ -2012,10 +2012,10 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2041,8 +2041,8 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
@@ -2066,8 +2066,8 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
@@ -2091,8 +2091,8 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="3" t="s">
         <v>33</v>
       </c>
@@ -2116,8 +2116,8 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="3" t="s">
         <v>34</v>
       </c>
@@ -2141,8 +2141,8 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="3" t="s">
         <v>35</v>
       </c>
@@ -2166,8 +2166,8 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="3" t="s">
         <v>39</v>
       </c>
@@ -2191,8 +2191,8 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="3" t="s">
         <v>40</v>
       </c>
@@ -2216,8 +2216,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
@@ -2241,7 +2241,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="13"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
@@ -2268,10 +2268,10 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2297,8 +2297,8 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="3" t="s">
         <v>28</v>
       </c>
@@ -2322,8 +2322,8 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="3" t="s">
         <v>29</v>
       </c>
@@ -2347,8 +2347,8 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="3" t="s">
         <v>33</v>
       </c>
@@ -2372,8 +2372,8 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="3" t="s">
         <v>34</v>
       </c>
@@ -2397,8 +2397,8 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="3" t="s">
         <v>35</v>
       </c>
@@ -2422,8 +2422,8 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="3" t="s">
         <v>39</v>
       </c>
@@ -2447,8 +2447,8 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="3" t="s">
         <v>40</v>
       </c>
@@ -2472,8 +2472,8 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="3" t="s">
         <v>41</v>
       </c>
@@ -2497,7 +2497,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="13"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
@@ -2524,10 +2524,10 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2553,8 +2553,8 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="12"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="3" t="s">
         <v>55</v>
       </c>
@@ -2578,8 +2578,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="12"/>
-      <c r="B39" s="11" t="s">
+      <c r="A39" s="11"/>
+      <c r="B39" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2605,8 +2605,8 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="3" t="s">
         <v>25</v>
       </c>
@@ -2630,10 +2630,10 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2659,8 +2659,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="14"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="3" t="s">
         <v>57</v>
       </c>
@@ -2684,8 +2684,8 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14" t="s">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2711,8 +2711,8 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="3" t="s">
         <v>37</v>
       </c>
@@ -2736,10 +2736,10 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2765,8 +2765,8 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="14"/>
-      <c r="B46" s="16"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="14"/>
       <c r="C46" s="3" t="s">
         <v>57</v>
       </c>
@@ -2790,8 +2790,8 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -2817,8 +2817,8 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
       <c r="C48" s="3" t="s">
         <v>38</v>
       </c>
@@ -2842,10 +2842,10 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2871,8 +2871,8 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
       <c r="C50" s="3" t="s">
         <v>60</v>
       </c>
@@ -2896,15 +2896,17 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="12"/>
-      <c r="B51" s="13"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="12"/>
       <c r="C51" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D51" s="2">
         <v>2</v>
       </c>
-      <c r="E51" s="2"/>
+      <c r="E51" s="2">
+        <v>0</v>
+      </c>
       <c r="F51" s="2">
         <f>D51*2</f>
         <v>4</v>
@@ -2919,8 +2921,8 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="12"/>
-      <c r="B52" s="11" t="s">
+      <c r="A52" s="11"/>
+      <c r="B52" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2946,8 +2948,8 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
       <c r="C53" s="3" t="s">
         <v>55</v>
       </c>
@@ -2971,10 +2973,10 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -3000,8 +3002,8 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="14"/>
-      <c r="B55" s="17" t="s">
+      <c r="A55" s="9"/>
+      <c r="B55" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -3027,10 +3029,10 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -3056,8 +3058,8 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17" t="s">
+      <c r="A57" s="9"/>
+      <c r="B57" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -3084,11 +3086,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B27:B35"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="B17:B25"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B47:B48"/>
@@ -3098,19 +3108,11 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A49:A53"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add event for logistics process
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -966,31 +966,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1373,7 +1373,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1577,8 +1577,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1619,10 +1620,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1648,8 +1649,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="17"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1673,8 +1674,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="17"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1700,8 +1701,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1725,8 +1726,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1750,10 +1751,10 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1779,8 +1780,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="17"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1804,87 +1805,87 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="17"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="2">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="E9" s="2">
         <f>H9</f>
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="2">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" ref="E10:E11" si="3">H10</f>
-        <v>5000</v>
+        <v>25000</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="2">
-        <v>200</v>
+        <v>1250</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>12500</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>2500</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1910,8 +1911,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="17"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1935,164 +1936,164 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="17"/>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="E14" s="2">
         <f>H14</f>
-        <v>10000</v>
+        <v>40000</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" ref="E15:E16" si="4">H15</f>
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="4"/>
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="6">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="E17" s="6">
         <v>0</v>
       </c>
       <c r="F17" s="2">
         <f>D17*2</f>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="6">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="6">
         <v>0</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ref="F18:F25" si="5">D18*2</f>
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="6">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E19" s="6">
         <v>0</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="5"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="3" t="s">
         <v>33</v>
       </c>
@@ -2116,8 +2117,8 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="3" t="s">
         <v>34</v>
       </c>
@@ -2141,8 +2142,8 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="3" t="s">
         <v>35</v>
       </c>
@@ -2166,82 +2167,82 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="6">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="E23" s="6">
         <v>0</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="5"/>
-        <v>16000</v>
+        <v>8000</v>
       </c>
       <c r="G23" s="6">
         <f t="shared" si="0"/>
-        <v>16000</v>
+        <v>8000</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="1"/>
-        <v>80000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="6">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="E24" s="6">
         <v>0</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="5"/>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="G24" s="6">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="6">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="E25" s="6">
         <v>0</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="5"/>
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="G25" s="6">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="1"/>
-        <v>25000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="12"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
@@ -2268,10 +2269,10 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2297,8 +2298,8 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="3" t="s">
         <v>28</v>
       </c>
@@ -2322,8 +2323,8 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="3" t="s">
         <v>29</v>
       </c>
@@ -2347,8 +2348,8 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="3" t="s">
         <v>33</v>
       </c>
@@ -2372,8 +2373,8 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="3" t="s">
         <v>34</v>
       </c>
@@ -2397,8 +2398,8 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="3" t="s">
         <v>35</v>
       </c>
@@ -2422,8 +2423,8 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="3" t="s">
         <v>39</v>
       </c>
@@ -2447,8 +2448,8 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="3" t="s">
         <v>40</v>
       </c>
@@ -2472,8 +2473,8 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="11"/>
-      <c r="B35" s="12"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="3" t="s">
         <v>41</v>
       </c>
@@ -2497,7 +2498,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="12"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
@@ -2524,37 +2525,37 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D37" s="2">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E37" s="2">
         <v>0</v>
       </c>
       <c r="F37" s="2">
         <f>D37*2</f>
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="G37" s="2">
         <f>D37*2</f>
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="H37" s="2">
         <f>G37*5</f>
-        <v>3000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="11"/>
-      <c r="B38" s="16"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="3" t="s">
         <v>55</v>
       </c>
@@ -2578,8 +2579,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10" t="s">
+      <c r="A39" s="13"/>
+      <c r="B39" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2605,8 +2606,8 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="3" t="s">
         <v>25</v>
       </c>
@@ -2630,10 +2631,10 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2659,8 +2660,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="9"/>
-      <c r="B42" s="14"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="3" t="s">
         <v>57</v>
       </c>
@@ -2684,62 +2685,62 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9" t="s">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D43" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E43" s="2">
         <f>H43</f>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" si="12"/>
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D44" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" ref="E44" si="13">H44</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" si="11"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" si="12"/>
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2765,8 +2766,8 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="9"/>
-      <c r="B46" s="14"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="3" t="s">
         <v>57</v>
       </c>
@@ -2790,62 +2791,62 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9" t="s">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D47" s="2">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E47" s="2">
         <f>H47</f>
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="15"/>
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D48" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" ref="E48" si="16">H48</f>
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" si="14"/>
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" si="15"/>
-        <v>100</v>
+        <v>400</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2871,8 +2872,8 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="3" t="s">
         <v>60</v>
       </c>
@@ -2896,8 +2897,8 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="11"/>
-      <c r="B51" s="12"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="14"/>
       <c r="C51" s="3" t="s">
         <v>61</v>
       </c>
@@ -2921,8 +2922,8 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="11"/>
-      <c r="B52" s="10" t="s">
+      <c r="A52" s="13"/>
+      <c r="B52" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2948,8 +2949,8 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
       <c r="C53" s="3" t="s">
         <v>55</v>
       </c>
@@ -2973,7 +2974,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="15" t="s">
         <v>62</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3002,7 +3003,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="9"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="8" t="s">
         <v>26</v>
       </c>
@@ -3029,7 +3030,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="15" t="s">
         <v>65</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -3058,7 +3059,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="9"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="8" t="s">
         <v>26</v>
       </c>
@@ -3086,19 +3087,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A49:A53"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B47:B48"/>
@@ -3108,11 +3101,19 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B27:B35"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add more info to daily log
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="3" r:id="rId1"/>
@@ -83,18 +83,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>192.168.1.10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>db_user</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>hello123456</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>仓库</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -283,6 +275,14 @@
   </si>
   <si>
     <t>冷轧厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>test123456</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>localhost</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -938,7 +938,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -964,6 +964,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1352,14 +1358,14 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
+      <c r="C2" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1372,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1577,9 +1583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1598,36 +1604,36 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
@@ -1649,10 +1655,10 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2">
         <v>50</v>
@@ -1674,12 +1680,12 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="10"/>
-      <c r="B4" s="9" t="s">
-        <v>26</v>
+      <c r="A4" s="12"/>
+      <c r="B4" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2">
         <v>2000</v>
@@ -1689,7 +1695,7 @@
         <v>20000</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
@@ -1701,10 +1707,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2">
         <v>1000</v>
@@ -1714,7 +1720,7 @@
         <v>10000</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
@@ -1726,10 +1732,10 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2">
         <v>500</v>
@@ -1739,7 +1745,7 @@
         <v>5000</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
@@ -1751,14 +1757,14 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>23</v>
+      <c r="A7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2">
         <v>10</v>
@@ -1780,10 +1786,10 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
@@ -1805,12 +1811,12 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="10"/>
-      <c r="B9" s="9" t="s">
-        <v>26</v>
+      <c r="A9" s="12"/>
+      <c r="B9" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2">
         <v>5000</v>
@@ -1820,7 +1826,7 @@
         <v>50000</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
@@ -1832,10 +1838,10 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" s="2">
         <v>2500</v>
@@ -1845,7 +1851,7 @@
         <v>25000</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
@@ -1857,10 +1863,10 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2">
         <v>1250</v>
@@ -1870,7 +1876,7 @@
         <v>12500</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
@@ -1882,14 +1888,14 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>23</v>
+      <c r="A12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2">
         <v>10</v>
@@ -1911,10 +1917,10 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2">
         <v>5</v>
@@ -1936,12 +1942,12 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="10"/>
-      <c r="B14" s="9" t="s">
-        <v>26</v>
+      <c r="A14" s="12"/>
+      <c r="B14" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2">
         <v>4000</v>
@@ -1951,7 +1957,7 @@
         <v>40000</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
@@ -1963,10 +1969,10 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2">
         <v>2000</v>
@@ -1976,7 +1982,7 @@
         <v>20000</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
@@ -1988,10 +1994,10 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2">
         <v>1000</v>
@@ -2001,7 +2007,7 @@
         <v>10000</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
@@ -2013,14 +2019,14 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>23</v>
+      <c r="A17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" s="6">
         <v>2000</v>
@@ -2042,10 +2048,10 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" s="6">
         <v>1000</v>
@@ -2067,10 +2073,10 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19" s="6">
         <v>500</v>
@@ -2092,10 +2098,10 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="6">
         <v>5000</v>
@@ -2117,10 +2123,10 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D21" s="6">
         <v>2500</v>
@@ -2142,10 +2148,10 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D22" s="6">
         <v>1250</v>
@@ -2167,10 +2173,10 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="6">
         <v>4000</v>
@@ -2192,10 +2198,10 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" s="6">
         <v>2000</v>
@@ -2217,10 +2223,10 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25" s="6">
         <v>1000</v>
@@ -2242,12 +2248,12 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="14"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
@@ -2257,7 +2263,7 @@
         <v>20</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="0"/>
@@ -2269,14 +2275,14 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>23</v>
+      <c r="A27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D27" s="6">
         <v>2500</v>
@@ -2298,10 +2304,10 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D28" s="6">
         <v>1500</v>
@@ -2323,10 +2329,10 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D29" s="6">
         <v>1500</v>
@@ -2348,10 +2354,10 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D30" s="6">
         <v>3000</v>
@@ -2373,10 +2379,10 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D31" s="6">
         <v>4000</v>
@@ -2398,10 +2404,10 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D32" s="6">
         <v>1000</v>
@@ -2423,10 +2429,10 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D33" s="6">
         <v>4000</v>
@@ -2448,10 +2454,10 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D34" s="6">
         <v>3000</v>
@@ -2473,10 +2479,10 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="13"/>
-      <c r="B35" s="14"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D35" s="6">
         <v>2500</v>
@@ -2498,12 +2504,12 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="14"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D36" s="6">
         <v>20</v>
@@ -2513,7 +2519,7 @@
         <v>200</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G36" s="6">
         <f t="shared" si="6"/>
@@ -2525,14 +2531,14 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>23</v>
+      <c r="A37" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D37" s="2">
         <v>400</v>
@@ -2554,10 +2560,10 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="13"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D38" s="2">
         <v>100</v>
@@ -2579,12 +2585,12 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="13"/>
-      <c r="B39" s="12" t="s">
-        <v>26</v>
+      <c r="A39" s="15"/>
+      <c r="B39" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D39" s="2">
         <v>200</v>
@@ -2594,7 +2600,7 @@
         <v>2000</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" si="8"/>
@@ -2606,10 +2612,10 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D40" s="2">
         <v>100</v>
@@ -2619,7 +2625,7 @@
         <v>1000</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G40" s="2">
         <f t="shared" si="8"/>
@@ -2631,14 +2637,14 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>23</v>
+      <c r="A41" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D41" s="2">
         <v>100</v>
@@ -2660,10 +2666,10 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="15"/>
-      <c r="B42" s="17"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D42" s="2">
         <v>200</v>
@@ -2685,12 +2691,12 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15" t="s">
-        <v>26</v>
+      <c r="A43" s="17"/>
+      <c r="B43" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D43" s="2">
         <v>25</v>
@@ -2700,7 +2706,7 @@
         <v>250</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" si="11"/>
@@ -2712,10 +2718,10 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D44" s="2">
         <v>20</v>
@@ -2725,7 +2731,7 @@
         <v>200</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" si="11"/>
@@ -2737,14 +2743,14 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>23</v>
+      <c r="A45" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D45" s="2">
         <v>50</v>
@@ -2766,10 +2772,10 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="15"/>
-      <c r="B46" s="17"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D46" s="2">
         <v>100</v>
@@ -2791,12 +2797,12 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15" t="s">
-        <v>26</v>
+      <c r="A47" s="17"/>
+      <c r="B47" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D47" s="2">
         <v>50</v>
@@ -2806,7 +2812,7 @@
         <v>500</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" si="14"/>
@@ -2818,10 +2824,10 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D48" s="2">
         <v>40</v>
@@ -2831,7 +2837,7 @@
         <v>400</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" si="14"/>
@@ -2843,14 +2849,14 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>23</v>
+      <c r="A49" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D49" s="2">
         <v>10000</v>
@@ -2872,10 +2878,10 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D50" s="2">
         <v>300</v>
@@ -2897,10 +2903,10 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="13"/>
-      <c r="B51" s="14"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="16"/>
       <c r="C51" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D51" s="2">
         <v>2</v>
@@ -2922,12 +2928,12 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="13"/>
-      <c r="B52" s="12" t="s">
-        <v>26</v>
+      <c r="A52" s="15"/>
+      <c r="B52" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D52" s="2">
         <v>800</v>
@@ -2937,7 +2943,7 @@
         <v>8000</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G52" s="2">
         <f t="shared" si="17"/>
@@ -2949,10 +2955,10 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
       <c r="C53" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D53" s="2">
         <v>200</v>
@@ -2962,7 +2968,7 @@
         <v>2000</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G53" s="2">
         <f t="shared" si="17"/>
@@ -2974,14 +2980,14 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D54" s="2">
         <v>100</v>
@@ -3003,12 +3009,12 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="15"/>
+      <c r="A55" s="17"/>
       <c r="B55" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D55" s="2">
         <v>100</v>
@@ -3018,7 +3024,7 @@
         <v>1000</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G55" s="2">
         <f t="shared" ref="G55" si="21">D55*2</f>
@@ -3030,14 +3036,14 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="15" t="s">
-        <v>65</v>
+      <c r="A56" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D56" s="2">
         <v>100</v>
@@ -3059,12 +3065,12 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="15"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D57" s="2">
         <v>100</v>
@@ -3074,7 +3080,7 @@
         <v>1000</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G57" s="2">
         <f t="shared" ref="G57" si="24">D57*2</f>

</xml_diff>

<commit_message>
Add pause limit check
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="3" r:id="rId1"/>
@@ -972,14 +972,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -991,12 +985,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1378,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1583,9 +1583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1626,10 +1626,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1655,8 +1655,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1680,87 +1680,87 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="2">
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="E4" s="2">
         <f>H4</f>
-        <v>20000</v>
+        <v>80000</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>16000</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="2">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E6" si="2">H5</f>
-        <v>10000</v>
+        <v>40000</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="2">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>20000</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1786,8 +1786,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
@@ -1811,87 +1811,87 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="2">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="E9" s="2">
         <f>H9</f>
-        <v>50000</v>
+        <v>80000</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
-        <v>50000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="2">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" ref="E10:E11" si="3">H10</f>
-        <v>25000</v>
+        <v>40000</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
-        <v>25000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="2">
-        <v>1250</v>
+        <v>2000</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="3"/>
-        <v>12500</v>
+        <v>20000</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
-        <v>12500</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1917,8 +1917,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1942,164 +1942,164 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="12"/>
-      <c r="B14" s="11" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="2">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="E14" s="2">
         <f>H14</f>
-        <v>40000</v>
+        <v>80000</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>16000</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" ref="E15:E16" si="4">H15</f>
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="4"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="6">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="E17" s="6">
         <v>0</v>
       </c>
       <c r="F17" s="2">
         <f>D17*2</f>
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E18" s="6">
         <v>0</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" ref="F18:F25" si="5">D18*2</f>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="6">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E19" s="6">
         <v>0</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="3" t="s">
         <v>31</v>
       </c>
@@ -2123,8 +2123,8 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="3" t="s">
         <v>32</v>
       </c>
@@ -2148,8 +2148,8 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="3" t="s">
         <v>33</v>
       </c>
@@ -2173,8 +2173,8 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
@@ -2198,8 +2198,8 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="3" t="s">
         <v>38</v>
       </c>
@@ -2223,8 +2223,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="3" t="s">
         <v>39</v>
       </c>
@@ -2248,7 +2248,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="16"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
@@ -2275,62 +2275,62 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="6">
-        <v>2500</v>
+        <v>6000</v>
       </c>
       <c r="E27" s="6">
         <v>0</v>
       </c>
       <c r="F27" s="2">
         <f>D27*2</f>
-        <v>5000</v>
+        <v>12000</v>
       </c>
       <c r="G27" s="6">
         <f t="shared" ref="G27:G36" si="6">D27*2</f>
-        <v>5000</v>
+        <v>12000</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="1"/>
-        <v>25000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="6">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="E28" s="6">
         <v>0</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" ref="F28:F35" si="7">D28*2</f>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="G28" s="6">
         <f t="shared" si="6"/>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="3" t="s">
         <v>27</v>
       </c>
@@ -2354,58 +2354,58 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="6">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="E30" s="6">
         <v>0</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="7"/>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="G30" s="6">
         <f t="shared" si="6"/>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="6">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="E31" s="6">
         <v>0</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="7"/>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="G31" s="6">
         <f t="shared" si="6"/>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="3" t="s">
         <v>33</v>
       </c>
@@ -2429,82 +2429,82 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="6">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="E33" s="6">
         <v>0</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" si="7"/>
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="G33" s="6">
         <f t="shared" si="6"/>
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D34" s="6">
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="E34" s="6">
         <v>0</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" si="7"/>
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="G34" s="6">
         <f t="shared" si="6"/>
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D35" s="6">
-        <v>2500</v>
+        <v>1250</v>
       </c>
       <c r="E35" s="6">
         <v>0</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="7"/>
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="G35" s="6">
         <f t="shared" si="6"/>
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="1"/>
-        <v>25000</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="16"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="2" t="s">
         <v>24</v>
       </c>
@@ -2531,10 +2531,10 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2560,8 +2560,8 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="15"/>
-      <c r="B38" s="13"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="3" t="s">
         <v>53</v>
       </c>
@@ -2585,8 +2585,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="15"/>
-      <c r="B39" s="14" t="s">
+      <c r="A39" s="13"/>
+      <c r="B39" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2612,8 +2612,8 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="3" t="s">
         <v>23</v>
       </c>
@@ -2637,10 +2637,10 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2666,8 +2666,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="17"/>
-      <c r="B42" s="19"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="3" t="s">
         <v>55</v>
       </c>
@@ -2691,8 +2691,8 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2718,8 +2718,8 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="3" t="s">
         <v>35</v>
       </c>
@@ -2743,10 +2743,10 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2772,8 +2772,8 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="17"/>
-      <c r="B46" s="19"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="3" t="s">
         <v>55</v>
       </c>
@@ -2797,8 +2797,8 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17" t="s">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -2824,8 +2824,8 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
       <c r="C48" s="3" t="s">
         <v>36</v>
       </c>
@@ -2849,10 +2849,10 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2878,8 +2878,8 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="3" t="s">
         <v>58</v>
       </c>
@@ -2903,8 +2903,8 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="15"/>
-      <c r="B51" s="16"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="14"/>
       <c r="C51" s="3" t="s">
         <v>59</v>
       </c>
@@ -2928,8 +2928,8 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="15"/>
-      <c r="B52" s="14" t="s">
+      <c r="A52" s="13"/>
+      <c r="B52" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2955,8 +2955,8 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
       <c r="C53" s="3" t="s">
         <v>53</v>
       </c>
@@ -2980,7 +2980,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3009,7 +3009,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="17"/>
+      <c r="A55" s="11"/>
       <c r="B55" s="8" t="s">
         <v>24</v>
       </c>
@@ -3036,7 +3036,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -3065,7 +3065,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="17"/>
+      <c r="A57" s="11"/>
       <c r="B57" s="8" t="s">
         <v>24</v>
       </c>
@@ -3093,11 +3093,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B27:B35"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="B17:B25"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B47:B48"/>
@@ -3107,19 +3115,11 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A49:A53"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add dest id for event so that > 1 downstream factories can be used
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="3" r:id="rId1"/>
@@ -972,31 +972,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1378,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2">
         <v>2.2000000000000002</v>
@@ -1583,9 +1583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1626,10 +1626,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1655,8 +1655,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="19"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1680,87 +1680,87 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="19"/>
-      <c r="B4" s="17" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="2">
-        <v>8000</v>
+        <v>6000</v>
       </c>
       <c r="E4" s="2">
         <f>H4</f>
-        <v>80000</v>
+        <v>60000</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="1"/>
-        <v>80000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="2">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E6" si="2">H5</f>
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>6000</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="2">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="2"/>
-        <v>20000</v>
+        <v>15000</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1786,8 +1786,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="19"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
@@ -1811,87 +1811,87 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19"/>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="2">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="E9" s="2">
         <f>H9</f>
-        <v>80000</v>
+        <v>40000</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>16000</v>
+        <v>8000</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
-        <v>80000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="2">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" ref="E10:E11" si="3">H10</f>
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="3"/>
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1917,8 +1917,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="19"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1942,87 +1942,87 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="19"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="2">
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="E14" s="2">
         <f>H14</f>
-        <v>80000</v>
+        <v>50000</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>16000</v>
+        <v>10000</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
-        <v>80000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="2">
-        <v>4000</v>
+        <v>2500</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" ref="E15:E16" si="4">H15</f>
-        <v>40000</v>
+        <v>25000</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="2">
-        <v>2000</v>
+        <v>1250</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="4"/>
-        <v>20000</v>
+        <v>12500</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2500</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2048,8 +2048,8 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
@@ -2073,8 +2073,8 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
@@ -2098,8 +2098,8 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="3" t="s">
         <v>31</v>
       </c>
@@ -2123,8 +2123,8 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="3" t="s">
         <v>32</v>
       </c>
@@ -2148,8 +2148,8 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="3" t="s">
         <v>33</v>
       </c>
@@ -2173,8 +2173,8 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
@@ -2198,8 +2198,8 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="3" t="s">
         <v>38</v>
       </c>
@@ -2223,8 +2223,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="3" t="s">
         <v>39</v>
       </c>
@@ -2248,7 +2248,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="14"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
@@ -2275,10 +2275,10 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2304,8 +2304,8 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="3" t="s">
         <v>26</v>
       </c>
@@ -2329,8 +2329,8 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="3" t="s">
         <v>27</v>
       </c>
@@ -2354,8 +2354,8 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="3" t="s">
         <v>31</v>
       </c>
@@ -2379,8 +2379,8 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="3" t="s">
         <v>32</v>
       </c>
@@ -2404,8 +2404,8 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="3" t="s">
         <v>33</v>
       </c>
@@ -2429,8 +2429,8 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="3" t="s">
         <v>37</v>
       </c>
@@ -2454,8 +2454,8 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="3" t="s">
         <v>38</v>
       </c>
@@ -2479,8 +2479,8 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="13"/>
-      <c r="B35" s="14"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="3" t="s">
         <v>39</v>
       </c>
@@ -2504,7 +2504,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="14"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="2" t="s">
         <v>24</v>
       </c>
@@ -2531,10 +2531,10 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2560,8 +2560,8 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="13"/>
-      <c r="B38" s="18"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="3" t="s">
         <v>53</v>
       </c>
@@ -2585,8 +2585,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="13"/>
-      <c r="B39" s="12" t="s">
+      <c r="A39" s="15"/>
+      <c r="B39" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2612,8 +2612,8 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="3" t="s">
         <v>23</v>
       </c>
@@ -2637,10 +2637,10 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2666,8 +2666,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="11"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="3" t="s">
         <v>55</v>
       </c>
@@ -2691,8 +2691,8 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11" t="s">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2718,8 +2718,8 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="3" t="s">
         <v>35</v>
       </c>
@@ -2743,10 +2743,10 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="18" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2772,8 +2772,8 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="11"/>
-      <c r="B46" s="16"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="3" t="s">
         <v>55</v>
       </c>
@@ -2797,8 +2797,8 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11" t="s">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -2824,8 +2824,8 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="3" t="s">
         <v>36</v>
       </c>
@@ -2849,10 +2849,10 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2878,8 +2878,8 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="3" t="s">
         <v>58</v>
       </c>
@@ -2903,8 +2903,8 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="13"/>
-      <c r="B51" s="14"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="16"/>
       <c r="C51" s="3" t="s">
         <v>59</v>
       </c>
@@ -2928,8 +2928,8 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="13"/>
-      <c r="B52" s="12" t="s">
+      <c r="A52" s="15"/>
+      <c r="B52" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2955,8 +2955,8 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
       <c r="C53" s="3" t="s">
         <v>53</v>
       </c>
@@ -2980,7 +2980,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="17" t="s">
         <v>60</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3009,7 +3009,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="11"/>
+      <c r="A55" s="17"/>
       <c r="B55" s="8" t="s">
         <v>24</v>
       </c>
@@ -3036,7 +3036,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="17" t="s">
         <v>63</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -3065,7 +3065,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="11"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="8" t="s">
         <v>24</v>
       </c>
@@ -3093,19 +3093,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A49:A53"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B47:B48"/>
@@ -3115,11 +3107,19 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B27:B35"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add maintenance events and handling
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
   <si>
     <t>炼化厂</t>
   </si>
@@ -63,226 +63,234 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>飞机总装厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ip</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>username</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>db_user</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>仓库</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>原料库</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>聚氯乙烯</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>高苯聚氯乙烯</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成品库</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>塑料齿轮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>塑料连杆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>塑料外壳</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁质零件厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>热轧钢板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷轧钢板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁质齿轮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁质连杆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁质外壳</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝质零件厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>热轧铝板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷轧铝板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝质齿轮</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝质连杆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝质外壳</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>品名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>N/A</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始库存基数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>停产上/下限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进货下限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生产/消耗速度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞机</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>汽车</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始库存上限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞机总装厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>汽车总装厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>化工厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>苯</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>甲苯</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢锭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝锭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>炼化厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>原油</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>氢气</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>氧化铝（催化剂）</t>
+  </si>
+  <si>
+    <t>冶铁厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢锭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁矿石</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冶铝厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝矿石</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铝锭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>热轧厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷轧厂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>test123456</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>localhost</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>维修恢复时长（单位：时间周期）</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>飞机总装厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ip</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>username</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>password</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>db_user</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>仓库</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>原料库</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>聚氯乙烯</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>高苯聚氯乙烯</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>成品库</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>塑料齿轮</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>塑料连杆</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>塑料外壳</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铁质零件厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>热轧钢板</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冷轧钢板</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铁质齿轮</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铁质连杆</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铁质外壳</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铝质零件厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>热轧铝板</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冷轧铝板</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铝质齿轮</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铝质连杆</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铝质外壳</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>品名</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>N/A</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始库存基数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>停产上/下限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>进货下限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生产/消耗速度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>飞机</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>汽车</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始库存上限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>飞机总装厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>汽车总装厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>化工厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>苯</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>甲苯</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>钢锭</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铝锭</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>炼化厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>原油</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>氢气</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>氧化铝（催化剂）</t>
-  </si>
-  <si>
-    <t>冶铁厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>钢锭</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铁矿石</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冶铝厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铝矿石</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铝锭</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>热轧厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冷轧厂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>test123456</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>localhost</t>
+    <t>维修触发周期上限（单位：时间周期）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>维修触发周期下限（单位：时间周期）</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -938,7 +946,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -972,14 +980,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -991,12 +996,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1348,24 +1359,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1376,21 +1387,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="22.75" customWidth="1"/>
+    <col min="6" max="6" width="38.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1401,12 +1412,18 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1417,8 +1434,16 @@
       <c r="D2" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="11">
+        <f>D2*5</f>
+        <v>10</v>
+      </c>
+      <c r="F2" s="11">
+        <f>D2*10</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1431,8 +1456,16 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="11">
+        <f t="shared" ref="E3:E13" si="0">D3*5</f>
+        <v>5</v>
+      </c>
+      <c r="F3" s="11">
+        <f t="shared" ref="F3:F13" si="1">D3*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1445,8 +1478,16 @@
       <c r="D4" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1459,8 +1500,16 @@
       <c r="D5" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1473,8 +1522,16 @@
       <c r="D6" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1485,10 +1542,18 @@
         <v>1.2</v>
       </c>
       <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="F7" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1501,8 +1566,16 @@
       <c r="D8" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1515,8 +1588,16 @@
       <c r="D9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1527,10 +1608,18 @@
         <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1541,10 +1630,18 @@
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1555,10 +1652,18 @@
         <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1570,6 +1675,14 @@
       </c>
       <c r="D13" s="2">
         <v>1</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1604,36 +1717,36 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
@@ -1655,10 +1768,10 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>50</v>
@@ -1680,12 +1793,12 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="2">
         <v>6000</v>
@@ -1695,7 +1808,7 @@
         <v>60000</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
@@ -1707,10 +1820,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2">
         <v>3000</v>
@@ -1720,7 +1833,7 @@
         <v>30000</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
@@ -1732,10 +1845,10 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2">
         <v>1500</v>
@@ -1745,7 +1858,7 @@
         <v>15000</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
@@ -1757,14 +1870,14 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D7" s="2">
         <v>10</v>
@@ -1786,10 +1899,10 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2">
         <v>5</v>
@@ -1811,12 +1924,12 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11" t="s">
-        <v>24</v>
+      <c r="A9" s="20"/>
+      <c r="B9" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2">
         <v>4000</v>
@@ -1826,7 +1939,7 @@
         <v>40000</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
@@ -1838,10 +1951,10 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2">
         <v>2000</v>
@@ -1851,7 +1964,7 @@
         <v>20000</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
@@ -1863,10 +1976,10 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2">
         <v>1000</v>
@@ -1876,7 +1989,7 @@
         <v>10000</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
@@ -1888,14 +2001,14 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D12" s="2">
         <v>10</v>
@@ -1917,10 +2030,10 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2">
         <v>5</v>
@@ -1942,12 +2055,12 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="12"/>
-      <c r="B14" s="11" t="s">
-        <v>24</v>
+      <c r="A14" s="20"/>
+      <c r="B14" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2">
         <v>5000</v>
@@ -1957,7 +2070,7 @@
         <v>50000</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
@@ -1969,10 +2082,10 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2">
         <v>2500</v>
@@ -1982,7 +2095,7 @@
         <v>25000</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
@@ -1994,10 +2107,10 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2">
         <v>1250</v>
@@ -2007,7 +2120,7 @@
         <v>12500</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
@@ -2019,14 +2132,14 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>21</v>
+      <c r="A17" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="6">
         <v>4000</v>
@@ -2048,10 +2161,10 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="6">
         <v>2000</v>
@@ -2073,10 +2186,10 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="6">
         <v>1000</v>
@@ -2098,10 +2211,10 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="6">
         <v>5000</v>
@@ -2123,10 +2236,10 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="6">
         <v>2500</v>
@@ -2148,10 +2261,10 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="6">
         <v>1250</v>
@@ -2173,10 +2286,10 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="6">
         <v>4000</v>
@@ -2198,10 +2311,10 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="6">
         <v>2000</v>
@@ -2223,10 +2336,10 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="6">
         <v>1000</v>
@@ -2248,12 +2361,12 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="16"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
@@ -2263,7 +2376,7 @@
         <v>20</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="0"/>
@@ -2275,14 +2388,14 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>21</v>
+      <c r="A27" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" s="6">
         <v>6000</v>
@@ -2304,10 +2417,10 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" s="6">
         <v>3000</v>
@@ -2329,10 +2442,10 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="6">
         <v>1500</v>
@@ -2354,10 +2467,10 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="6">
         <v>4000</v>
@@ -2379,10 +2492,10 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="6">
         <v>2000</v>
@@ -2404,10 +2517,10 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
       <c r="C32" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="6">
         <v>1000</v>
@@ -2429,10 +2542,10 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D33" s="6">
         <v>5000</v>
@@ -2454,10 +2567,10 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D34" s="6">
         <v>2500</v>
@@ -2479,10 +2592,10 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
       <c r="C35" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35" s="6">
         <v>1250</v>
@@ -2504,12 +2617,12 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="16"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D36" s="6">
         <v>20</v>
@@ -2519,7 +2632,7 @@
         <v>200</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G36" s="6">
         <f t="shared" si="6"/>
@@ -2531,14 +2644,14 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D37" s="2">
         <v>400</v>
@@ -2560,10 +2673,10 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="15"/>
-      <c r="B38" s="13"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D38" s="2">
         <v>100</v>
@@ -2585,12 +2698,12 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="15"/>
-      <c r="B39" s="14" t="s">
-        <v>24</v>
+      <c r="A39" s="14"/>
+      <c r="B39" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="2">
         <v>200</v>
@@ -2600,7 +2713,7 @@
         <v>2000</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" si="8"/>
@@ -2612,10 +2725,10 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D40" s="2">
         <v>100</v>
@@ -2625,7 +2738,7 @@
         <v>1000</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G40" s="2">
         <f t="shared" si="8"/>
@@ -2637,14 +2750,14 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>21</v>
+      <c r="A41" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D41" s="2">
         <v>100</v>
@@ -2666,10 +2779,10 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="17"/>
-      <c r="B42" s="19"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D42" s="2">
         <v>200</v>
@@ -2691,12 +2804,12 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17" t="s">
-        <v>24</v>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D43" s="2">
         <v>25</v>
@@ -2706,7 +2819,7 @@
         <v>250</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" si="11"/>
@@ -2718,10 +2831,10 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" s="2">
         <v>20</v>
@@ -2731,7 +2844,7 @@
         <v>200</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" si="11"/>
@@ -2743,14 +2856,14 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>21</v>
+      <c r="A45" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D45" s="2">
         <v>50</v>
@@ -2772,10 +2885,10 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="17"/>
-      <c r="B46" s="19"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" s="2">
         <v>100</v>
@@ -2797,12 +2910,12 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17" t="s">
-        <v>24</v>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D47" s="2">
         <v>50</v>
@@ -2812,7 +2925,7 @@
         <v>500</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" si="14"/>
@@ -2824,10 +2937,10 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
       <c r="C48" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D48" s="2">
         <v>40</v>
@@ -2837,7 +2950,7 @@
         <v>400</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" si="14"/>
@@ -2849,14 +2962,14 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D49" s="2">
         <v>10000</v>
@@ -2878,10 +2991,10 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
       <c r="C50" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D50" s="2">
         <v>300</v>
@@ -2903,10 +3016,10 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="15"/>
-      <c r="B51" s="16"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="15"/>
       <c r="C51" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D51" s="2">
         <v>2</v>
@@ -2928,12 +3041,12 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="15"/>
-      <c r="B52" s="14" t="s">
-        <v>24</v>
+      <c r="A52" s="14"/>
+      <c r="B52" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52" s="2">
         <v>800</v>
@@ -2943,7 +3056,7 @@
         <v>8000</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G52" s="2">
         <f t="shared" si="17"/>
@@ -2955,10 +3068,10 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
       <c r="C53" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53" s="2">
         <v>200</v>
@@ -2968,7 +3081,7 @@
         <v>2000</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G53" s="2">
         <f t="shared" si="17"/>
@@ -2980,14 +3093,14 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="17" t="s">
-        <v>60</v>
+      <c r="A54" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D54" s="2">
         <v>100</v>
@@ -3009,12 +3122,12 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="17"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D55" s="2">
         <v>100</v>
@@ -3024,7 +3137,7 @@
         <v>1000</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G55" s="2">
         <f t="shared" ref="G55" si="21">D55*2</f>
@@ -3036,14 +3149,14 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D56" s="2">
         <v>100</v>
@@ -3065,12 +3178,12 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="17"/>
+      <c r="A57" s="12"/>
       <c r="B57" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D57" s="2">
         <v>100</v>
@@ -3080,7 +3193,7 @@
         <v>1000</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G57" s="2">
         <f t="shared" ref="G57" si="24">D57*2</f>
@@ -3093,11 +3206,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B27:B35"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="B17:B25"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B47:B48"/>
@@ -3107,19 +3228,11 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A49:A53"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add power consumption handling
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -10,13 +10,14 @@
     <sheet name="database" sheetId="3" r:id="rId1"/>
     <sheet name="factory" sheetId="1" r:id="rId2"/>
     <sheet name="stocks" sheetId="2" r:id="rId3"/>
+    <sheet name="power_station" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
   <si>
     <t>炼化厂</t>
   </si>
@@ -291,6 +292,22 @@
   </si>
   <si>
     <t>维修触发周期下限（单位：时间周期）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>居民区</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>波动范围</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>发电预测上限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>总发电量下限</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -946,7 +963,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -983,6 +1000,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1008,6 +1028,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1387,21 +1410,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="22.75" customWidth="1"/>
-    <col min="6" max="6" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="25.375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="24.125" customWidth="1"/>
+    <col min="7" max="7" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1420,8 +1446,11 @@
       <c r="F1" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1442,8 +1471,11 @@
         <f>D2*10</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1464,8 +1496,11 @@
         <f t="shared" ref="F3:F13" si="1">D3*10</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1486,8 +1521,11 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1508,8 +1546,11 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1530,8 +1571,11 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1552,8 +1596,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1574,8 +1621,11 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1596,8 +1646,11 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1618,8 +1671,11 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1640,8 +1696,11 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1662,8 +1721,11 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="22">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1683,6 +1745,32 @@
       <c r="F13" s="11">
         <f t="shared" si="1"/>
         <v>10</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="6">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="22">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -1697,8 +1785,8 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1739,10 +1827,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1768,8 +1856,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="20"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
@@ -1793,8 +1881,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="20"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1820,8 +1908,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1845,8 +1933,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1870,10 +1958,10 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1899,8 +1987,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
@@ -1924,8 +2012,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="20"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1951,8 +2039,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1976,8 +2064,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
@@ -2001,10 +2089,10 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -2030,8 +2118,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="20"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
@@ -2055,8 +2143,8 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="20"/>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -2082,8 +2170,8 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
@@ -2107,8 +2195,8 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
@@ -2132,10 +2220,10 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2161,8 +2249,8 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
@@ -2186,8 +2274,8 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
@@ -2211,8 +2299,8 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
@@ -2236,8 +2324,8 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
@@ -2261,8 +2349,8 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
@@ -2286,8 +2374,8 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="3" t="s">
         <v>36</v>
       </c>
@@ -2311,8 +2399,8 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="3" t="s">
         <v>37</v>
       </c>
@@ -2336,8 +2424,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="3" t="s">
         <v>38</v>
       </c>
@@ -2361,7 +2449,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="15"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
@@ -2388,10 +2476,10 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2417,8 +2505,8 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="3" t="s">
         <v>25</v>
       </c>
@@ -2442,8 +2530,8 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="3" t="s">
         <v>26</v>
       </c>
@@ -2467,8 +2555,8 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="3" t="s">
         <v>30</v>
       </c>
@@ -2492,8 +2580,8 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="3" t="s">
         <v>31</v>
       </c>
@@ -2517,8 +2605,8 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="3" t="s">
         <v>32</v>
       </c>
@@ -2542,8 +2630,8 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="3" t="s">
         <v>36</v>
       </c>
@@ -2567,8 +2655,8 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="3" t="s">
         <v>37</v>
       </c>
@@ -2592,8 +2680,8 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="3" t="s">
         <v>38</v>
       </c>
@@ -2617,7 +2705,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="15"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="2" t="s">
         <v>23</v>
       </c>
@@ -2644,10 +2732,10 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2673,8 +2761,8 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="14"/>
-      <c r="B38" s="19"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="3" t="s">
         <v>52</v>
       </c>
@@ -2698,8 +2786,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="14"/>
-      <c r="B39" s="13" t="s">
+      <c r="A39" s="15"/>
+      <c r="B39" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2725,8 +2813,8 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="3" t="s">
         <v>22</v>
       </c>
@@ -2750,10 +2838,10 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2779,8 +2867,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="12"/>
-      <c r="B42" s="17"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="3" t="s">
         <v>54</v>
       </c>
@@ -2804,8 +2892,8 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12" t="s">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2831,8 +2919,8 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="3" t="s">
         <v>34</v>
       </c>
@@ -2856,10 +2944,10 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2885,8 +2973,8 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="12"/>
-      <c r="B46" s="17"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="3" t="s">
         <v>54</v>
       </c>
@@ -2910,8 +2998,8 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12" t="s">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -2937,8 +3025,8 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="3" t="s">
         <v>35</v>
       </c>
@@ -2962,10 +3050,10 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2991,8 +3079,8 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="3" t="s">
         <v>57</v>
       </c>
@@ -3016,8 +3104,8 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="14"/>
-      <c r="B51" s="15"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="16"/>
       <c r="C51" s="3" t="s">
         <v>58</v>
       </c>
@@ -3041,8 +3129,8 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="14"/>
-      <c r="B52" s="13" t="s">
+      <c r="A52" s="15"/>
+      <c r="B52" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -3068,8 +3156,8 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="15"/>
-      <c r="B53" s="15"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
       <c r="C53" s="3" t="s">
         <v>52</v>
       </c>
@@ -3093,7 +3181,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="13" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3122,7 +3210,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="12"/>
+      <c r="A55" s="13"/>
       <c r="B55" s="8" t="s">
         <v>23</v>
       </c>
@@ -3149,7 +3237,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="12" t="s">
+      <c r="A56" s="13" t="s">
         <v>62</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -3178,7 +3266,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="12"/>
+      <c r="A57" s="13"/>
       <c r="B57" s="8" t="s">
         <v>23</v>
       </c>
@@ -3237,4 +3325,40 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add attack handling, and specific process for power station
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -10,14 +10,13 @@
     <sheet name="database" sheetId="3" r:id="rId1"/>
     <sheet name="factory" sheetId="1" r:id="rId2"/>
     <sheet name="stocks" sheetId="2" r:id="rId3"/>
-    <sheet name="power_station" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
   <si>
     <t>炼化厂</t>
   </si>
@@ -300,14 +299,6 @@
   </si>
   <si>
     <t>波动范围</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>发电预测上限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>总发电量下限</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1000,38 +991,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1413,14 +1404,14 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="3" max="3" width="24.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="24.125" customWidth="1"/>
@@ -1458,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -1471,7 +1462,7 @@
         <f>D2*10</f>
         <v>20</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1483,20 +1474,20 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="11">
-        <f t="shared" ref="E3:E13" si="0">D3*5</f>
+        <f t="shared" ref="E3:E12" si="0">D3*5</f>
         <v>5</v>
       </c>
       <c r="F3" s="11">
-        <f t="shared" ref="F3:F13" si="1">D3*10</f>
+        <f t="shared" ref="F3:F12" si="1">D3*10</f>
         <v>10</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1508,7 +1499,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>2.2000000000000002</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -1521,7 +1512,7 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1546,7 +1537,7 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1571,7 +1562,7 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1583,7 +1574,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1596,7 +1587,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1608,7 +1599,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="2">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
@@ -1621,7 +1612,7 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1633,7 +1624,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -1646,7 +1637,7 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1658,7 +1649,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
@@ -1671,7 +1662,7 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1683,7 +1674,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
@@ -1696,7 +1687,7 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="12">
         <v>0.05</v>
       </c>
     </row>
@@ -1708,7 +1699,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
@@ -1721,53 +1712,54 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="12">
         <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="6">
+        <v>5</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <v>2</v>
       </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C14" s="2">
+        <f>SUMPRODUCT((B2:B13),(C2:C13))/B14</f>
+        <v>27.5</v>
+      </c>
+      <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E13" s="11">
-        <f t="shared" si="0"/>
+      <c r="E14" s="11">
+        <f>D14*5</f>
         <v>5</v>
       </c>
-      <c r="F13" s="11">
-        <f t="shared" si="1"/>
+      <c r="F14" s="11">
+        <f>D14*10</f>
         <v>10</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="6">
-        <v>6</v>
-      </c>
-      <c r="C14" s="6">
-        <v>2</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="G14" s="22">
         <v>0.1</v>
@@ -1827,10 +1819,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1856,8 +1848,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="21"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
@@ -1881,8 +1873,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="21"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1908,8 +1900,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1933,8 +1925,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1958,10 +1950,10 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1987,8 +1979,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="21"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
@@ -2012,8 +2004,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="21"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -2039,8 +2031,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
@@ -2064,8 +2056,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
@@ -2089,10 +2081,10 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -2118,8 +2110,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="21"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
@@ -2143,8 +2135,8 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="21"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -2170,8 +2162,8 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
@@ -2195,8 +2187,8 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
@@ -2220,10 +2212,10 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2249,8 +2241,8 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
@@ -2274,8 +2266,8 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
@@ -2299,8 +2291,8 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
@@ -2324,8 +2316,8 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
@@ -2349,8 +2341,8 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
@@ -2374,8 +2366,8 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="3" t="s">
         <v>36</v>
       </c>
@@ -2399,8 +2391,8 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="3" t="s">
         <v>37</v>
       </c>
@@ -2424,8 +2416,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="3" t="s">
         <v>38</v>
       </c>
@@ -2449,7 +2441,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="16"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
@@ -2476,10 +2468,10 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2505,8 +2497,8 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="3" t="s">
         <v>25</v>
       </c>
@@ -2530,8 +2522,8 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="3" t="s">
         <v>26</v>
       </c>
@@ -2555,8 +2547,8 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="3" t="s">
         <v>30</v>
       </c>
@@ -2580,8 +2572,8 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="3" t="s">
         <v>31</v>
       </c>
@@ -2605,8 +2597,8 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="3" t="s">
         <v>32</v>
       </c>
@@ -2630,8 +2622,8 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="3" t="s">
         <v>36</v>
       </c>
@@ -2655,8 +2647,8 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="3" t="s">
         <v>37</v>
       </c>
@@ -2680,8 +2672,8 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="18"/>
       <c r="C35" s="3" t="s">
         <v>38</v>
       </c>
@@ -2705,7 +2697,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="16"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="2" t="s">
         <v>23</v>
       </c>
@@ -2732,10 +2724,10 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2761,8 +2753,8 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="15"/>
-      <c r="B38" s="20"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="3" t="s">
         <v>52</v>
       </c>
@@ -2786,8 +2778,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="15"/>
-      <c r="B39" s="14" t="s">
+      <c r="A39" s="17"/>
+      <c r="B39" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2813,8 +2805,8 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
       <c r="C40" s="3" t="s">
         <v>22</v>
       </c>
@@ -2838,10 +2830,10 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2867,8 +2859,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="13"/>
-      <c r="B42" s="18"/>
+      <c r="A42" s="19"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="3" t="s">
         <v>54</v>
       </c>
@@ -2892,8 +2884,8 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13" t="s">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2919,8 +2911,8 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="3" t="s">
         <v>34</v>
       </c>
@@ -2944,10 +2936,10 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2973,8 +2965,8 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="13"/>
-      <c r="B46" s="18"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="21"/>
       <c r="C46" s="3" t="s">
         <v>54</v>
       </c>
@@ -2998,8 +2990,8 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13" t="s">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -3025,8 +3017,8 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
       <c r="C48" s="3" t="s">
         <v>35</v>
       </c>
@@ -3050,10 +3042,10 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -3079,8 +3071,8 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="3" t="s">
         <v>57</v>
       </c>
@@ -3104,8 +3096,8 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="15"/>
-      <c r="B51" s="16"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="18"/>
       <c r="C51" s="3" t="s">
         <v>58</v>
       </c>
@@ -3129,8 +3121,8 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="15"/>
-      <c r="B52" s="14" t="s">
+      <c r="A52" s="17"/>
+      <c r="B52" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -3156,8 +3148,8 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
       <c r="C53" s="3" t="s">
         <v>52</v>
       </c>
@@ -3181,7 +3173,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3210,7 +3202,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="13"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="8" t="s">
         <v>23</v>
       </c>
@@ -3237,7 +3229,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -3266,7 +3258,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="13"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="8" t="s">
         <v>23</v>
       </c>
@@ -3294,19 +3286,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A49:A53"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B47:B48"/>
@@ -3316,49 +3300,21 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B27:B35"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="B2" s="12">
-        <v>0.2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
handle the case when power supply is insufficient
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -994,14 +994,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1013,16 +1010,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1747,8 +1747,8 @@
         <v>2</v>
       </c>
       <c r="C14" s="2">
-        <f>SUMPRODUCT((B2:B13),(C2:C13))/B14</f>
-        <v>27.5</v>
+        <f>SUMPRODUCT((B2:B13),(C2:C13))/B14*0.9</f>
+        <v>24.75</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
@@ -1761,7 +1761,7 @@
         <f>D14*10</f>
         <v>10</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="13">
         <v>0.1</v>
       </c>
     </row>
@@ -1777,7 +1777,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
@@ -1819,10 +1819,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1848,8 +1848,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
@@ -1873,8 +1873,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="14"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="20" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1900,8 +1900,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1925,8 +1925,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1950,10 +1950,10 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1979,8 +1979,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
@@ -2004,8 +2004,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="14"/>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="20" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -2031,8 +2031,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
@@ -2056,8 +2056,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
@@ -2081,10 +2081,10 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -2110,8 +2110,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
@@ -2135,8 +2135,8 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="14"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="20" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -2162,8 +2162,8 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
@@ -2187,8 +2187,8 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
@@ -2212,10 +2212,10 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2241,8 +2241,8 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
@@ -2266,8 +2266,8 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
@@ -2291,8 +2291,8 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
@@ -2316,8 +2316,8 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
@@ -2341,8 +2341,8 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
@@ -2366,8 +2366,8 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="3" t="s">
         <v>36</v>
       </c>
@@ -2391,8 +2391,8 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="3" t="s">
         <v>37</v>
       </c>
@@ -2416,8 +2416,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="17"/>
-      <c r="B25" s="18"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="3" t="s">
         <v>38</v>
       </c>
@@ -2441,7 +2441,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="18"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
@@ -2468,10 +2468,10 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2497,8 +2497,8 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="3" t="s">
         <v>25</v>
       </c>
@@ -2522,8 +2522,8 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="3" t="s">
         <v>26</v>
       </c>
@@ -2547,8 +2547,8 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="3" t="s">
         <v>30</v>
       </c>
@@ -2572,8 +2572,8 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="3" t="s">
         <v>31</v>
       </c>
@@ -2597,8 +2597,8 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="3" t="s">
         <v>32</v>
       </c>
@@ -2622,8 +2622,8 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="3" t="s">
         <v>36</v>
       </c>
@@ -2647,8 +2647,8 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="3" t="s">
         <v>37</v>
       </c>
@@ -2672,8 +2672,8 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="17"/>
-      <c r="B35" s="18"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="3" t="s">
         <v>38</v>
       </c>
@@ -2697,7 +2697,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="18"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="2" t="s">
         <v>23</v>
       </c>
@@ -2724,10 +2724,10 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2753,8 +2753,8 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="17"/>
-      <c r="B38" s="15"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="21"/>
       <c r="C38" s="3" t="s">
         <v>52</v>
       </c>
@@ -2778,8 +2778,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="17"/>
-      <c r="B39" s="16" t="s">
+      <c r="A39" s="16"/>
+      <c r="B39" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2805,8 +2805,8 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
       <c r="C40" s="3" t="s">
         <v>22</v>
       </c>
@@ -2830,10 +2830,10 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2859,8 +2859,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="19"/>
-      <c r="B42" s="21"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="3" t="s">
         <v>54</v>
       </c>
@@ -2884,8 +2884,8 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19" t="s">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2911,8 +2911,8 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="3" t="s">
         <v>34</v>
       </c>
@@ -2936,10 +2936,10 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2965,8 +2965,8 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="19"/>
-      <c r="B46" s="21"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="3" t="s">
         <v>54</v>
       </c>
@@ -2990,8 +2990,8 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19" t="s">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -3017,8 +3017,8 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
       <c r="C48" s="3" t="s">
         <v>35</v>
       </c>
@@ -3042,10 +3042,10 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -3071,8 +3071,8 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
       <c r="C50" s="3" t="s">
         <v>57</v>
       </c>
@@ -3096,8 +3096,8 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="17"/>
-      <c r="B51" s="18"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="3" t="s">
         <v>58</v>
       </c>
@@ -3121,8 +3121,8 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="17"/>
-      <c r="B52" s="16" t="s">
+      <c r="A52" s="16"/>
+      <c r="B52" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -3148,8 +3148,8 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
       <c r="C53" s="3" t="s">
         <v>52</v>
       </c>
@@ -3173,7 +3173,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3202,7 +3202,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="19"/>
+      <c r="A55" s="14"/>
       <c r="B55" s="8" t="s">
         <v>23</v>
       </c>
@@ -3229,7 +3229,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -3258,7 +3258,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="19"/>
+      <c r="A57" s="14"/>
       <c r="B57" s="8" t="s">
         <v>23</v>
       </c>
@@ -3286,11 +3286,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A27:A36"/>
+    <mergeCell ref="B27:B35"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="B17:B25"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B47:B48"/>
@@ -3300,19 +3308,11 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A27:A36"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A49:A53"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adjust maintenance period limit
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="3" r:id="rId1"/>
@@ -290,11 +290,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>10.10.2.42</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sim_engine</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>localhost</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -950,7 +950,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -989,6 +989,12 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1357,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1380,11 +1386,11 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>71</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>72</v>
       </c>
       <c r="C2" s="9">
         <v>123456</v>
@@ -1400,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1452,12 +1458,12 @@
         <v>2</v>
       </c>
       <c r="E2" s="10">
-        <f>D2*5</f>
-        <v>10</v>
+        <f>D2*20</f>
+        <v>40</v>
       </c>
       <c r="F2" s="10">
-        <f>D2*10</f>
-        <v>20</v>
+        <f>D2*30</f>
+        <v>60</v>
       </c>
       <c r="G2" s="11">
         <v>0.05</v>
@@ -1476,13 +1482,13 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" ref="E3:E12" si="0">D3*5</f>
-        <v>5</v>
-      </c>
-      <c r="F3" s="10">
-        <f t="shared" ref="F3:F12" si="1">D3*10</f>
-        <v>10</v>
+      <c r="E3" s="15">
+        <f t="shared" ref="E3:E14" si="0">D3*20</f>
+        <v>20</v>
+      </c>
+      <c r="F3" s="15">
+        <f t="shared" ref="F3:F14" si="1">D3*30</f>
+        <v>30</v>
       </c>
       <c r="G3" s="11">
         <v>0.05</v>
@@ -1493,19 +1499,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="2">
-        <v>3</v>
-      </c>
-      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F4" s="10">
+        <v>20</v>
+      </c>
+      <c r="F4" s="15">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
@@ -1524,15 +1530,15 @@
         <v>2.5</v>
       </c>
       <c r="D5" s="2">
-        <v>3</v>
-      </c>
-      <c r="E5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="15">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F5" s="10">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="F5" s="15">
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
       <c r="G5" s="11">
         <v>0.05</v>
@@ -1549,13 +1555,13 @@
         <v>2.5</v>
       </c>
       <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="15">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F6" s="10">
+        <v>20</v>
+      </c>
+      <c r="F6" s="15">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
@@ -1574,15 +1580,15 @@
         <v>2</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10">
+        <v>2</v>
+      </c>
+      <c r="E7" s="15">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F7" s="10">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>40</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
       <c r="G7" s="11">
         <v>0.05</v>
@@ -1599,15 +1605,15 @@
         <v>2</v>
       </c>
       <c r="D8" s="2">
-        <v>2</v>
-      </c>
-      <c r="E8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F8" s="10">
-        <f t="shared" si="1"/>
         <v>20</v>
+      </c>
+      <c r="F8" s="15">
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="G8" s="11">
         <v>0.05</v>
@@ -1624,15 +1630,15 @@
         <v>2</v>
       </c>
       <c r="D9" s="2">
-        <v>2</v>
-      </c>
-      <c r="E9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F9" s="10">
-        <f t="shared" si="1"/>
         <v>20</v>
+      </c>
+      <c r="F9" s="15">
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="G9" s="11">
         <v>0.05</v>
@@ -1649,15 +1655,15 @@
         <v>1.5</v>
       </c>
       <c r="D10" s="2">
-        <v>2</v>
-      </c>
-      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F10" s="10">
-        <f t="shared" si="1"/>
         <v>20</v>
+      </c>
+      <c r="F10" s="15">
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="G10" s="11">
         <v>0.05</v>
@@ -1674,15 +1680,15 @@
         <v>2</v>
       </c>
       <c r="D11" s="2">
-        <v>2</v>
-      </c>
-      <c r="E11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F11" s="10">
-        <f t="shared" si="1"/>
         <v>20</v>
+      </c>
+      <c r="F11" s="15">
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="G11" s="11">
         <v>0.05</v>
@@ -1699,15 +1705,15 @@
         <v>1.5</v>
       </c>
       <c r="D12" s="2">
-        <v>2</v>
-      </c>
-      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F12" s="10">
-        <f t="shared" si="1"/>
         <v>20</v>
+      </c>
+      <c r="F12" s="15">
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="G12" s="11">
         <v>0.05</v>
@@ -1745,18 +1751,18 @@
       </c>
       <c r="C14" s="2">
         <f>SUMPRODUCT((B2:B13),(C2:C13))/B14*0.9</f>
-        <v>24.75</v>
+        <v>23.400000000000002</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="10">
-        <f>D14*5</f>
-        <v>5</v>
-      </c>
-      <c r="F14" s="10">
-        <f>D14*10</f>
-        <v>10</v>
+      <c r="E14" s="15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F14" s="15">
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="G14" s="12">
         <v>0.1</v>
@@ -1816,10 +1822,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1845,8 +1851,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1870,8 +1876,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="15"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1897,8 +1903,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1922,8 +1928,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1947,10 +1953,10 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1976,8 +1982,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
@@ -2001,8 +2007,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="15"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -2028,8 +2034,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
@@ -2053,8 +2059,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="3" t="s">
         <v>31</v>
       </c>
@@ -2078,10 +2084,10 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -2107,8 +2113,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="3" t="s">
         <v>34</v>
       </c>
@@ -2132,8 +2138,8 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -2159,8 +2165,8 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
@@ -2184,8 +2190,8 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
@@ -2209,10 +2215,10 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2238,8 +2244,8 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="3" t="s">
         <v>24</v>
       </c>
@@ -2263,8 +2269,8 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
@@ -2288,8 +2294,8 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
@@ -2313,8 +2319,8 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="3" t="s">
         <v>30</v>
       </c>
@@ -2338,8 +2344,8 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="3" t="s">
         <v>31</v>
       </c>
@@ -2363,8 +2369,8 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="3" t="s">
         <v>35</v>
       </c>
@@ -2388,8 +2394,8 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="3" t="s">
         <v>36</v>
       </c>
@@ -2413,8 +2419,8 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="3" t="s">
         <v>37</v>
       </c>
@@ -2438,7 +2444,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
@@ -2465,10 +2471,10 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2494,8 +2500,8 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="3" t="s">
         <v>24</v>
       </c>
@@ -2519,8 +2525,8 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="3" t="s">
         <v>25</v>
       </c>
@@ -2544,8 +2550,8 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="3" t="s">
         <v>29</v>
       </c>
@@ -2569,8 +2575,8 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="3" t="s">
         <v>30</v>
       </c>
@@ -2594,8 +2600,8 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="3" t="s">
         <v>31</v>
       </c>
@@ -2619,8 +2625,8 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="3" t="s">
         <v>35</v>
       </c>
@@ -2644,8 +2650,8 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="3" t="s">
         <v>36</v>
       </c>
@@ -2669,8 +2675,8 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="3" t="s">
         <v>37</v>
       </c>
@@ -2694,7 +2700,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="19"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="2" t="s">
         <v>22</v>
       </c>
@@ -2721,10 +2727,10 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2750,8 +2756,8 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="18"/>
-      <c r="B38" s="16"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="3" t="s">
         <v>51</v>
       </c>
@@ -2775,8 +2781,8 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="18"/>
-      <c r="B39" s="17" t="s">
+      <c r="A39" s="20"/>
+      <c r="B39" s="19" t="s">
         <v>22</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2802,8 +2808,8 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
       <c r="C40" s="3" t="s">
         <v>21</v>
       </c>
@@ -2827,10 +2833,10 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2856,8 +2862,8 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="20"/>
-      <c r="B42" s="22"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="3" t="s">
         <v>53</v>
       </c>
@@ -2881,8 +2887,8 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20" t="s">
+      <c r="A43" s="22"/>
+      <c r="B43" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2908,8 +2914,8 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="3" t="s">
         <v>33</v>
       </c>
@@ -2933,10 +2939,10 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2962,8 +2968,8 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="20"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="3" t="s">
         <v>53</v>
       </c>
@@ -2987,8 +2993,8 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20" t="s">
+      <c r="A47" s="22"/>
+      <c r="B47" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -3014,8 +3020,8 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="3" t="s">
         <v>34</v>
       </c>
@@ -3039,10 +3045,10 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -3068,8 +3074,8 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
       <c r="C50" s="3" t="s">
         <v>56</v>
       </c>
@@ -3093,8 +3099,8 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="21"/>
       <c r="C51" s="3" t="s">
         <v>57</v>
       </c>
@@ -3118,8 +3124,8 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="18"/>
-      <c r="B52" s="17" t="s">
+      <c r="A52" s="20"/>
+      <c r="B52" s="19" t="s">
         <v>22</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -3145,8 +3151,8 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
       <c r="C53" s="3" t="s">
         <v>51</v>
       </c>
@@ -3170,7 +3176,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="20" t="s">
+      <c r="A54" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3199,7 +3205,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="20"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="8" t="s">
         <v>22</v>
       </c>
@@ -3226,7 +3232,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="22" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -3255,7 +3261,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="20"/>
+      <c r="A57" s="22"/>
       <c r="B57" s="8" t="s">
         <v>22</v>
       </c>

</xml_diff>